<commit_message>
Adding the first 2 points of CYRS review Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/Review.xlsx
+++ b/Input Documents/Review.xlsx
@@ -4,18 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="CYRS review" sheetId="1" r:id="rId1"/>
-    <sheet name="HSI review" sheetId="4" r:id="rId2"/>
+    <sheet name="Review" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
   <si>
     <t>Review point</t>
   </si>
@@ -102,6 +101,19 @@
   <si>
     <t xml:space="preserve">In Features section:
 3rd feature is called "TI" --&gt; Turn indicator not "T1"
+</t>
+  </si>
+  <si>
+    <t>24/1/2021</t>
+  </si>
+  <si>
+    <t>LED String-CYRS</t>
+  </si>
+  <si>
+    <t>24/1/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Block diagram isn't correct, it shall be a block has input signals(Tail signal - right TI signal - left TI signal - Mode signal) and has outputs (LEDs)
 </t>
   </si>
 </sst>
@@ -167,7 +179,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="21">
     <dxf>
       <font>
         <condense val="0"/>
@@ -334,128 +346,6 @@
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
       </font>
     </dxf>
   </dxfs>
@@ -748,28 +638,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="59" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -908,17 +786,39 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+    <row r="9" spans="1:5" ht="30">
+      <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="60">
+      <c r="A10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1"/>
@@ -1088,7 +988,7 @@
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
+  <conditionalFormatting sqref="E8:E10">
     <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
@@ -1100,7 +1000,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Edit Review sheet, Review the solved points and open new points Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/Review.xlsx
+++ b/Input Documents/Review.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Review" sheetId="4" r:id="rId1"/>
+    <sheet name="HSI" sheetId="4" r:id="rId1"/>
+    <sheet name="CYRS" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="29">
   <si>
     <t>Review point</t>
   </si>
@@ -35,12 +36,6 @@
   </si>
   <si>
     <t>Open</t>
-  </si>
-  <si>
-    <t>Document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIQ sheet </t>
   </si>
   <si>
     <t>Good job for the SIQ online form, but please provide a 
@@ -48,9 +43,6 @@
   </si>
   <si>
     <t>As mentioned in SIQ online form, startup animation modes are according to input signal called "Mode" provided by input switch "Mode switch" so fig.1 shall be updated to indicate that you have an input switch.</t>
-  </si>
-  <si>
-    <t>LED String-HSI</t>
   </si>
   <si>
     <t>Output LEDs shall be more declared in the block diagram: 
@@ -107,14 +99,47 @@
     <t>24/1/2021</t>
   </si>
   <si>
-    <t>LED String-CYRS</t>
-  </si>
-  <si>
     <t>24/1/2022</t>
   </si>
   <si>
     <t xml:space="preserve">Block diagram isn't correct, it shall be a block has input signals(Tail signal - right TI signal - left TI signal - Mode signal) and has outputs (LEDs)
 </t>
+  </si>
+  <si>
+    <t>Acceptance</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Mali 30/1/2020: Point is closed</t>
+  </si>
+  <si>
+    <t>Mali 30/1/2020: Still open</t>
+  </si>
+  <si>
+    <t>30/1/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version 1.0.1 shall be 1.1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inblock diagram please add 2 switches for TI function (Right TI and Let TI)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI output LEDs name is wrong it's written "T1 LEDs"
+</t>
+  </si>
+  <si>
+    <t>There are no requirements in CYRS</t>
   </si>
 </sst>
 </file>
@@ -158,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -175,11 +200,754 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="107">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -638,21 +1406,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59" customWidth="1"/>
+    <col min="3" max="3" width="59" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -660,197 +1429,224 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="45">
+      <c r="F1" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="45">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30">
+        <v>20</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="60">
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="60">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>10</v>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="60">
+        <v>20</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="60">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="6"/>
       <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="30">
+      <c r="F5" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>13</v>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="210">
+        <v>20</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="210">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>14</v>
+      <c r="D7" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45">
+        <v>20</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>17</v>
+      <c r="C8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30">
+        <v>20</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="C9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="6"/>
       <c r="E9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="60">
+    <row r="10" spans="1:6" ht="45">
       <c r="A10" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="C10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="6"/>
       <c r="E10" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:5">
+    <row r="11" spans="1:6" ht="30">
+      <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -933,78 +1729,210 @@
       <c r="D30" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E3">
-    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Open">
+  <conditionalFormatting sqref="E2:E8">
+    <cfRule type="containsText" dxfId="54" priority="33" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="53" priority="34" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="52" priority="35" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Closed">
-      <formula>NOT(ISERROR(SEARCH("Closed",E4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E4)))</formula>
+  <conditionalFormatting sqref="D2:D8">
+    <cfRule type="cellIs" dxfId="51" priority="16" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="17" operator="equal">
+      <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Closed">
-      <formula>NOT(ISERROR(SEARCH("Closed",E5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="containsText" dxfId="49" priority="13" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="14" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="15" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Closed">
-      <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="43" priority="11" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="12" operator="equal">
+      <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Closed">
-      <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="containsText" dxfId="39" priority="8" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="9" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="10" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8:E10">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Closed">
-      <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="cellIs" dxfId="33" priority="6" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="7" operator="equal">
+      <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10">
+  <conditionalFormatting sqref="E11">
+    <cfRule type="containsText" dxfId="29" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="4" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="5" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11">
       <formula1>"Open, Closed"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D11">
+      <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="60">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E2:E4">
+    <cfRule type="containsText" dxfId="59" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="4" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="57" priority="5" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D3">
+    <cfRule type="cellIs" dxfId="56" priority="1" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="2" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
+      <formula1>"Accepted, Rejected"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4">
+      <formula1>"Open, Closed"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Review the updated CYRS and close 2 opened points Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/Review.xlsx
+++ b/Input Documents/Review.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="40">
   <si>
     <t>Review point</t>
   </si>
@@ -140,6 +140,52 @@
   </si>
   <si>
     <t>There are no requirements in CYRS</t>
+  </si>
+  <si>
+    <t>Mali 30/1/2020: Still open
+Mali 31/1/2020: Still open</t>
+  </si>
+  <si>
+    <t>31/1/2020</t>
+  </si>
+  <si>
+    <t>In Document history table version 1.1 the comment is
+"Adding requirements" isn't descriptive enough</t>
+  </si>
+  <si>
+    <t>Layout of the system shall be like the HSI block diagram
+LEDs only are not the system, the system is input switches, controller and output LEDs</t>
+  </si>
+  <si>
+    <t>TI requirements don't declare that when right/left TI is activated (R1 to R6 / L1 to L6), the scenario of activation shall be repeated.
+Also the animation shall be declared that from R1 to R6 shall be :
+R1
+R1 + R2
+R1+R2+R3
+…etc, then OFF all LEDs, then repeat again till TI signal is LOW</t>
+  </si>
+  <si>
+    <t>Mali 31/1/2020: Point is reviewed and closed</t>
+  </si>
+  <si>
+    <t>Mali 30/1/2020: Still open
+Mali 31/1/2020: Point is reviewed and closed</t>
+  </si>
+  <si>
+    <t>For every animation (Mode1, Mode2 and TI activation), requirements don't declare the timing between every LED.
+So please provide as a system engineer a timing between every LED activation to have an animation.</t>
+  </si>
+  <si>
+    <t>HSI shall describe the used HW components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSI shall describe every usage of microcontroller pin, for ex: Pin 30 assigned to R1.
+So please provide a table that decalres:
+Pin number, it's direction (o/p - i/p) and assigned for what </t>
+  </si>
+  <si>
+    <t>Remove the status (proposed) from the doc. Name 
+"LED_STRING_ANIMATION_CYRS_proposed"</t>
   </si>
 </sst>
 </file>
@@ -213,7 +259,45 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="107">
+  <dxfs count="60">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -242,25 +326,6 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -390,44 +455,6 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -452,6 +479,25 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -495,25 +541,6 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -538,6 +565,25 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -581,25 +627,6 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -624,6 +651,25 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -704,392 +750,6 @@
         <condense val="0"/>
         <extend val="0"/>
         <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
@@ -1408,8 +1068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1623,16 +1283,34 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="A12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="60">
+      <c r="A13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1"/>
@@ -1730,86 +1408,124 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E8">
-    <cfRule type="containsText" dxfId="54" priority="33" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="59" priority="43" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="34" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="58" priority="44" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="35" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="57" priority="45" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D8">
-    <cfRule type="cellIs" dxfId="51" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="26" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="27" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="49" priority="13" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="54" priority="23" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="14" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="53" priority="24" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="15" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="52" priority="25" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="43" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="21" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="22" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
+    <cfRule type="containsText" dxfId="49" priority="18" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="19" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="20" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="cellIs" dxfId="46" priority="16" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="17" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="containsText" dxfId="44" priority="13" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="14" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="15" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="41" priority="11" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="12" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
     <cfRule type="containsText" dxfId="39" priority="8" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="38" priority="9" operator="containsText" text="Closed">
-      <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Closed",E12)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="37" priority="10" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="33" priority="6" operator="equal">
+      <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
-    <cfRule type="containsText" dxfId="29" priority="3" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="4" operator="containsText" text="Closed">
-      <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="5" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+  <conditionalFormatting sqref="E13">
+    <cfRule type="containsText" dxfId="34" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="4" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="5" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E13">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D13">
       <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1820,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1869,8 +1585,8 @@
       <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>23</v>
+      <c r="F2" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="60">
@@ -1883,12 +1599,14 @@
       <c r="C3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="E3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1901,35 +1619,192 @@
       <c r="C4" s="7" t="s">
         <v>28</v>
       </c>
+      <c r="D4" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="E4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30">
+      <c r="A5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:6" ht="60">
+      <c r="A6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="150">
+      <c r="A7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="75">
+      <c r="A8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30">
+      <c r="A9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E4">
-    <cfRule type="containsText" dxfId="59" priority="3" operator="containsText" text="Open">
+  <conditionalFormatting sqref="E2:E5">
+    <cfRule type="containsText" dxfId="29" priority="23" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="4" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="28" priority="24" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D3">
-    <cfRule type="cellIs" dxfId="56" priority="1" operator="equal">
+  <conditionalFormatting sqref="D2:D5">
+    <cfRule type="cellIs" dxfId="26" priority="21" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="22" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="containsText" dxfId="24" priority="18" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="21" priority="16" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="17" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="containsText" dxfId="14" priority="8" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9">
       <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E9">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update Review sheet or CYRS & HSI Adding SRS review sheet Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/Review.xlsx
+++ b/Input Documents/Review.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA47937-776A-44AB-A2C9-414D8E258133}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="HSI" sheetId="4" r:id="rId1"/>
@@ -16,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="49">
   <si>
     <t>Review point</t>
   </si>
@@ -188,12 +187,46 @@
     <t>Remove the status (proposed) from the doc. Name 
 "LED_STRING_ANIMATION_CYRS_proposed"</t>
   </si>
+  <si>
+    <t>Mali 6/2/2020: Point is reviewed and closed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mali 6/2/2020: Please provide the animation 
+mode in more detailes don’t let the SRS developer to guess  the requirement.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't make the requirement as a section name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mali 6/2/2020: Please provide the animation 
+mode in more detailes.
+</t>
+  </si>
+  <si>
+    <t>4. Req_PO5_LSAN_ LED STRING ANIMATION_08_V01:
+shall be "When left TI" not "When right TI"</t>
+  </si>
+  <si>
+    <t>Mali 30/1/2020: Still open
+Mali 6/2/2020: Point is closed</t>
+  </si>
+  <si>
+    <t>Mali 6/2/2020: Point is closed</t>
+  </si>
+  <si>
+    <t>Mali 6/2/2020: Still open</t>
+  </si>
+  <si>
+    <t>Mali 6/2/2020: there is still a amissing colom the
+assignation for every pin</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -256,11 +289,428 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="103">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -736,14 +1186,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -790,7 +1232,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -822,27 +1264,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -874,24 +1298,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1067,23 +1473,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.81640625" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1103,7 +1509,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="45">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1123,7 +1529,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1133,15 +1539,17 @@
       <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="E3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="60">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1161,7 +1569,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="60">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1179,7 +1587,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="30">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1199,7 +1607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="210">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -1219,7 +1627,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="45">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -1239,7 +1647,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="30">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -1249,12 +1657,17 @@
       <c r="C9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="E9" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -1268,8 +1681,11 @@
       <c r="E10" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="F10" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
@@ -1283,8 +1699,11 @@
       <c r="E11" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F11" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
@@ -1299,7 +1718,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="60">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
@@ -1313,221 +1732,243 @@
       <c r="E13" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F13" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E8">
-    <cfRule type="containsText" dxfId="54" priority="43" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="102" priority="48" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="44" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="101" priority="49" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="45" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="100" priority="50" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D8">
-    <cfRule type="cellIs" dxfId="51" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="31" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="32" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="49" priority="23" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="97" priority="28" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="24" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="96" priority="29" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="25" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="95" priority="30" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="46" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="26" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="27" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="containsText" dxfId="44" priority="18" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="92" priority="23" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="19" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="91" priority="24" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="20" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="90" priority="25" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="41" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="21" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="22" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="containsText" dxfId="39" priority="13" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="87" priority="18" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="14" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="86" priority="19" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="15" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="85" priority="20" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="36" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="16" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="17" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="containsText" dxfId="34" priority="8" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="82" priority="13" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="9" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="81" priority="14" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="10" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="80" priority="15" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="31" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="11" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="12" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="containsText" dxfId="29" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="77" priority="8" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="4" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="76" priority="9" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="75" priority="10" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="6" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="7" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E13" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E13">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D13" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D13">
       <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1537,23 +1978,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.81640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.26953125" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1573,7 +2014,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="30">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -1583,9 +2024,7 @@
       <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="D2" s="6"/>
       <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1593,7 +2032,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="60">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1613,7 +2052,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1633,7 +2072,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="30">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
@@ -1647,10 +2086,13 @@
         <v>19</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="60">
       <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
@@ -1664,10 +2106,13 @@
         <v>19</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="145" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="150">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
@@ -1677,14 +2122,15 @@
       <c r="C7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="D7" s="6"/>
       <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="F7" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="75">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
@@ -1694,14 +2140,15 @@
       <c r="C8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="D8" s="6"/>
       <c r="E8" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="F8" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30">
       <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
@@ -1715,110 +2162,180 @@
         <v>19</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="9">
+        <v>43984</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="3" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="11" spans="1:6" ht="30">
+      <c r="A11" s="10">
+        <v>43984</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E5">
-    <cfRule type="containsText" dxfId="24" priority="23" operator="containsText" text="Open">
+  <conditionalFormatting sqref="E2:E6">
+    <cfRule type="containsText" dxfId="72" priority="33" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="71" priority="34" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="25" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="70" priority="35" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D5">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+  <conditionalFormatting sqref="D2:D6">
+    <cfRule type="cellIs" dxfId="69" priority="31" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="32" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="67" priority="28" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="66" priority="29" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="65" priority="30" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="26" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="27" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="62" priority="23" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="61" priority="24" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="60" priority="25" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="21" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="22" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="57" priority="18" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="56" priority="19" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="55" priority="20" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="16" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="17" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="52" priority="13" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="51" priority="14" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="50" priority="15" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="11" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="12" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E10:E11">
+    <cfRule type="containsText" dxfId="37" priority="8" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="9" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="10" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="cellIs" dxfId="31" priority="6" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="5" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D10">
       <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E9" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update review sheet Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/Review.xlsx
+++ b/Input Documents/Review.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="53">
   <si>
     <t>Review point</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Mali 30/1/2020: Point is closed</t>
   </si>
   <si>
-    <t>Mali 30/1/2020: Still open</t>
-  </si>
-  <si>
     <t>30/1/2020</t>
   </si>
   <si>
@@ -140,10 +137,6 @@
   </si>
   <si>
     <t>There are no requirements in CYRS</t>
-  </si>
-  <si>
-    <t>Mali 30/1/2020: Still open
-Mali 31/1/2020: Still open</t>
   </si>
   <si>
     <t>31/1/2020</t>
@@ -191,35 +184,60 @@
     <t>Mali 6/2/2020: Point is reviewed and closed</t>
   </si>
   <si>
+    <t xml:space="preserve">Don't make the requirement as a section name </t>
+  </si>
+  <si>
+    <t>4. Req_PO5_LSAN_ LED STRING ANIMATION_08_V01:
+shall be "When left TI" not "When right TI"</t>
+  </si>
+  <si>
+    <t>Mali 30/1/2020: Still open
+Mali 6/2/2020: Point is closed</t>
+  </si>
+  <si>
+    <t>Mali 6/2/2020: Point is closed</t>
+  </si>
+  <si>
+    <t>Mali 30/1/2020: Still open
+Mali 9/2/2020: Point is closed</t>
+  </si>
+  <si>
+    <t>Mali 9/2/2020: Point is closed</t>
+  </si>
+  <si>
+    <t>Left TI animation mode declaration is wrong
+Req_PO5_LSAN_ LED STRING ANIMATION_07_V02</t>
+  </si>
+  <si>
+    <t>Mode 1 description is totally wrong</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mali 6/2/2020: Please provide the animation 
 mode in more detailes don’t let the SRS developer to guess  the requirement.
+Mali 9/2/2020: Point is closed
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Don't make the requirement as a section name </t>
   </si>
   <si>
     <t xml:space="preserve">Mali 6/2/2020: Please provide the animation 
 mode in more detailes.
+Mali 9/2/2020: Point is closed
 </t>
   </si>
   <si>
-    <t>4. Req_PO5_LSAN_ LED STRING ANIMATION_08_V01:
-shall be "When left TI" not "When right TI"</t>
+    <t>Mali 9/2/2020: Point is reviewed and closed</t>
   </si>
   <si>
     <t>Mali 30/1/2020: Still open
-Mali 6/2/2020: Point is closed</t>
-  </si>
-  <si>
-    <t>Mali 6/2/2020: Point is closed</t>
-  </si>
-  <si>
-    <t>Mali 6/2/2020: Still open</t>
+Mali 31/1/2020: Still open
+Mali 9/2/2020: Point is closed</t>
   </si>
   <si>
     <t>Mali 6/2/2020: there is still a amissing colom the
-assignation for every pin</t>
+assignation for every pin
+Mali 9/2/2020: still open</t>
+  </si>
+  <si>
+    <t>Mali 9/2/2020: still open</t>
   </si>
 </sst>
 </file>
@@ -299,306 +317,1816 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="103">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
+  <dxfs count="279">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
       </font>
     </dxf>
     <dxf>
@@ -1477,7 +3005,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1546,7 +3074,7 @@
         <v>20</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="60">
@@ -1579,12 +3107,14 @@
       <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="E5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30">
@@ -1649,13 +3179,13 @@
     </row>
     <row r="9" spans="1:6" ht="30">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>19</v>
@@ -1664,76 +3194,83 @@
         <v>20</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="45">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="E10" s="3" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30">
       <c r="A11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="6"/>
+        <v>26</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="E11" s="3" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="F12" s="7" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="60">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1832,135 +3369,230 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E8">
-    <cfRule type="containsText" dxfId="102" priority="48" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="278" priority="73" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="49" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="277" priority="74" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="50" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="276" priority="75" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D8">
-    <cfRule type="cellIs" dxfId="99" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="275" priority="56" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="274" priority="57" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="97" priority="28" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="273" priority="53" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="29" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="272" priority="54" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="30" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="271" priority="55" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="94" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="270" priority="51" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="269" priority="52" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="containsText" dxfId="92" priority="23" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="268" priority="48" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="24" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="267" priority="49" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="25" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="266" priority="50" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="89" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="265" priority="46" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="264" priority="47" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="containsText" dxfId="87" priority="18" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="263" priority="43" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="19" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="262" priority="44" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="20" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="261" priority="45" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="84" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="41" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="259" priority="42" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="containsText" dxfId="82" priority="13" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="258" priority="38" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="14" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="257" priority="39" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="15" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="256" priority="40" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="79" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="255" priority="36" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="37" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="containsText" dxfId="77" priority="8" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="253" priority="33" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="9" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="252" priority="34" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="10" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="251" priority="35" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="cellIs" dxfId="74" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="250" priority="31" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="249" priority="32" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="248" priority="28" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="247" priority="29" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="246" priority="30" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="26" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="244" priority="27" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="containsText" dxfId="203" priority="23" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="202" priority="24" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="201" priority="25" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="cellIs" dxfId="197" priority="21" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="196" priority="22" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="containsText" dxfId="193" priority="18" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="192" priority="19" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="191" priority="20" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="cellIs" dxfId="187" priority="16" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="186" priority="17" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="containsText" dxfId="183" priority="13" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="182" priority="14" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="181" priority="15" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="177" priority="11" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="176" priority="12" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="containsText" dxfId="173" priority="8" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="172" priority="9" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="171" priority="10" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="167" priority="6" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="166" priority="7" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="containsText" dxfId="163" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="162" priority="4" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="161" priority="5" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="157" priority="1" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="156" priority="2" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1979,10 +3611,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2014,7 +3646,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30">
+    <row r="2" spans="1:6" ht="45">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -2024,12 +3656,14 @@
       <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="E2" s="3" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="60">
@@ -2049,18 +3683,18 @@
         <v>20</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>19</v>
@@ -2069,18 +3703,18 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>19</v>
@@ -2089,18 +3723,18 @@
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="60">
       <c r="A6" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>19</v>
@@ -2109,54 +3743,58 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="150">
       <c r="A7" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="E7" s="3" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="75">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="6"/>
+        <v>34</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="E8" s="3" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30">
       <c r="A9" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>19</v>
@@ -2165,7 +3803,7 @@
         <v>20</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2176,11 +3814,16 @@
         <v>4</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="6"/>
+        <v>39</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="E10" s="3" t="s">
-        <v>6</v>
+        <v>20</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30">
@@ -2191,151 +3834,443 @@
         <v>4</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30">
+      <c r="A12" s="10">
+        <v>44076</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="10">
+        <v>44076</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E6">
-    <cfRule type="containsText" dxfId="72" priority="33" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="243" priority="101" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="34" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="242" priority="102" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="35" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="241" priority="103" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D6">
-    <cfRule type="cellIs" dxfId="69" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="99" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="100" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="67" priority="28" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="238" priority="96" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="29" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="237" priority="97" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="30" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="236" priority="98" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="64" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="94" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="234" priority="95" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="62" priority="23" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="233" priority="91" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="24" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="232" priority="92" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="25" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="231" priority="93" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="59" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="89" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="229" priority="90" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsText" dxfId="57" priority="18" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="228" priority="86" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="19" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="227" priority="87" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="20" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="226" priority="88" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="54" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="225" priority="84" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="85" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="52" priority="13" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="223" priority="81" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="14" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="222" priority="82" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="15" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="221" priority="83" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="49" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="79" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="80" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:E11">
-    <cfRule type="containsText" dxfId="37" priority="8" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="218" priority="76" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="9" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="217" priority="77" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="10" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="216" priority="78" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="31" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="74" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="75" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="213" priority="71" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="212" priority="72" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="211" priority="73" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="69" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="70" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="containsText" dxfId="153" priority="66" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="152" priority="67" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="151" priority="68" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="containsText" dxfId="147" priority="63" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="146" priority="64" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="145" priority="65" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="containsText" dxfId="141" priority="60" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="140" priority="61" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="139" priority="62" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="cellIs" dxfId="135" priority="58" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="134" priority="59" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="containsText" dxfId="131" priority="55" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="130" priority="56" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="129" priority="57" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="cellIs" dxfId="125" priority="53" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="124" priority="54" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="containsText" dxfId="121" priority="50" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="120" priority="51" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="119" priority="52" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="cellIs" dxfId="115" priority="48" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="49" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="containsText" dxfId="111" priority="45" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="110" priority="46" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="109" priority="47" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="cellIs" dxfId="105" priority="43" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="104" priority="44" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="containsText" dxfId="101" priority="40" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="100" priority="41" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="99" priority="42" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="cellIs" dxfId="95" priority="38" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="39" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="containsText" dxfId="91" priority="35" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="90" priority="36" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="89" priority="37" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="cellIs" dxfId="85" priority="33" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="34" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="containsText" dxfId="81" priority="30" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="80" priority="31" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="79" priority="32" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="cellIs" dxfId="75" priority="28" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="29" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="68" priority="26" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="27" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="containsText" dxfId="64" priority="23" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="63" priority="24" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="25" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="58" priority="21" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="22" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="containsText" dxfId="54" priority="18" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="53" priority="19" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="20" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="48" priority="16" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="17" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="containsText" dxfId="29" priority="13" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="14" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="15" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D11">
       <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E13">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update point 13 Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/Review.xlsx
+++ b/Input Documents/Review.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="53">
   <si>
     <t>Review point</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>Point status</t>
-  </si>
-  <si>
-    <t>Open</t>
   </si>
   <si>
     <t>Good job for the SIQ online form, but please provide a 
@@ -235,14 +232,15 @@
     <t>Mali 9/2/2020: still open</t>
   </si>
   <si>
+    <t>Mali 13/2/2020: Point is reviewed and closed</t>
+  </si>
+  <si>
     <t>Mali 6/2/2020: there is still a amissing colom the
 assignation for every pin
 Mali 9/2/2020: still open
 Mali 13/2/2020: there is still a amissing colom the
-assignation for every pin</t>
-  </si>
-  <si>
-    <t>Mali 13/2/2020: Point is reviewed and closed</t>
+assignation for every pin
+Mali 19/2/2020: Point is closed</t>
   </si>
 </sst>
 </file>
@@ -776,970 +774,970 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
       </font>
     </dxf>
     <dxf>
@@ -2876,7 +2874,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2899,13 +2897,13 @@
         <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45">
@@ -2916,36 +2914,36 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F2" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="60">
@@ -2956,16 +2954,16 @@
         <v>4</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F4" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60">
@@ -2976,16 +2974,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30">
@@ -2996,16 +2994,16 @@
         <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F6" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="210">
@@ -3016,16 +3014,16 @@
         <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F7" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="45">
@@ -3036,111 +3034,113 @@
         <v>4</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F8" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="45">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F10" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F11" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F12" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="75">
+    <row r="13" spans="1:6" ht="90">
       <c r="A13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="E13" s="3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>52</v>
@@ -3242,306 +3242,401 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E8">
-    <cfRule type="containsText" dxfId="262" priority="93" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="262" priority="118" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="261" priority="94" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="261" priority="119" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="260" priority="95" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="260" priority="120" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D8">
-    <cfRule type="cellIs" dxfId="259" priority="76" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="258" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="259" priority="101" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="258" priority="102" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="257" priority="73" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="257" priority="98" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="256" priority="74" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="256" priority="99" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="255" priority="75" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="255" priority="100" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="254" priority="71" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="253" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="96" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="253" priority="97" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="containsText" dxfId="252" priority="68" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="252" priority="93" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="251" priority="69" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="251" priority="94" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="250" priority="70" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="250" priority="95" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="249" priority="66" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="248" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="249" priority="91" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="248" priority="92" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="containsText" dxfId="247" priority="63" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="247" priority="88" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="246" priority="64" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="246" priority="89" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="245" priority="65" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="245" priority="90" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="244" priority="61" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="243" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="244" priority="86" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="243" priority="87" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="containsText" dxfId="242" priority="58" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="242" priority="83" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="241" priority="59" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="241" priority="84" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="240" priority="60" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="240" priority="85" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="239" priority="56" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="238" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="81" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="238" priority="82" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="containsText" dxfId="237" priority="53" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="237" priority="78" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="236" priority="54" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="236" priority="79" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="235" priority="55" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="235" priority="80" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="cellIs" dxfId="234" priority="51" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="233" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="234" priority="76" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="233" priority="77" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="232" priority="48" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="232" priority="73" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="231" priority="49" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="231" priority="74" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="230" priority="50" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="230" priority="75" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="229" priority="46" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="228" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="229" priority="71" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="228" priority="72" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="containsText" dxfId="227" priority="43" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="227" priority="68" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="226" priority="44" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="226" priority="69" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="225" priority="45" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="225" priority="70" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="224" priority="41" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="223" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="66" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="223" priority="67" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="containsText" dxfId="222" priority="38" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="222" priority="63" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="221" priority="39" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="221" priority="64" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="220" priority="40" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="220" priority="65" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="219" priority="36" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="218" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="61" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="218" priority="62" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="containsText" dxfId="217" priority="33" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="217" priority="58" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="216" priority="34" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="216" priority="59" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="215" priority="35" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="215" priority="60" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="214" priority="31" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="213" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="56" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="213" priority="57" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="containsText" dxfId="212" priority="28" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="212" priority="53" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="211" priority="29" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="211" priority="54" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="210" priority="30" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="210" priority="55" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="209" priority="26" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="208" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="51" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="208" priority="52" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="containsText" dxfId="207" priority="23" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="207" priority="48" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="206" priority="24" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="206" priority="49" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="205" priority="25" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="205" priority="50" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="204" priority="21" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="203" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="46" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="203" priority="47" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="containsText" dxfId="99" priority="18" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="202" priority="43" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="19" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="201" priority="44" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="20" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="200" priority="45" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="93" priority="16" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="41" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="198" priority="42" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="containsText" dxfId="89" priority="13" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="197" priority="38" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="14" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="196" priority="39" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="15" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="195" priority="40" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="83" priority="11" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="36" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="193" priority="37" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="containsText" dxfId="79" priority="8" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="192" priority="33" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="9" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="191" priority="34" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="10" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="190" priority="35" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="73" priority="6" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="31" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="188" priority="32" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="containsText" dxfId="69" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="187" priority="28" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="186" priority="29" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="185" priority="30" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="63" priority="1" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="26" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="183" priority="27" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="containsText" dxfId="49" priority="23" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="24" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="25" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="cellIs" dxfId="43" priority="21" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="22" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="containsText" dxfId="39" priority="18" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="19" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="20" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="cellIs" dxfId="33" priority="16" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="17" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="containsText" dxfId="29" priority="13" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="14" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="15" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3586,173 +3681,173 @@
         <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="60">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="60">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="150">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="75">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30">
       <c r="A9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3763,16 +3858,16 @@
         <v>4</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F10" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30">
@@ -3783,16 +3878,16 @@
         <v>4</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F11" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30">
@@ -3803,16 +3898,16 @@
         <v>4</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F12" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3823,521 +3918,521 @@
         <v>4</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F13" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E6">
-    <cfRule type="containsText" dxfId="202" priority="131" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="182" priority="131" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="201" priority="132" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="181" priority="132" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="200" priority="133" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="180" priority="133" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D6">
-    <cfRule type="cellIs" dxfId="199" priority="129" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="129" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="178" priority="130" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="197" priority="126" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="177" priority="126" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="196" priority="127" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="176" priority="127" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="195" priority="128" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="175" priority="128" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="194" priority="124" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="124" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="173" priority="125" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="192" priority="121" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="172" priority="121" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="191" priority="122" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="171" priority="122" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="190" priority="123" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="170" priority="123" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="189" priority="119" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="119" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="168" priority="120" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsText" dxfId="187" priority="116" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="167" priority="116" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="117" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="166" priority="117" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="185" priority="118" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="165" priority="118" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="184" priority="114" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="183" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="114" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="163" priority="115" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="182" priority="111" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="162" priority="111" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="112" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="161" priority="112" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="180" priority="113" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="160" priority="113" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="179" priority="109" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="109" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="158" priority="110" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:E11">
-    <cfRule type="containsText" dxfId="177" priority="106" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="157" priority="106" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="176" priority="107" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="156" priority="107" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="175" priority="108" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="155" priority="108" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="174" priority="104" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="104" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="153" priority="105" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="172" priority="101" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="152" priority="101" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="171" priority="102" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="151" priority="102" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="170" priority="103" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="150" priority="103" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="169" priority="99" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="168" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="99" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="148" priority="100" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="containsText" dxfId="167" priority="96" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="147" priority="96" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="97" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="146" priority="97" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="98" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="145" priority="98" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="containsText" dxfId="164" priority="93" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="144" priority="93" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="163" priority="94" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="143" priority="94" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="95" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="142" priority="95" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="161" priority="90" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="141" priority="90" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="91" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="140" priority="91" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="92" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="139" priority="92" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="158" priority="88" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="88" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="137" priority="89" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="156" priority="85" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="136" priority="85" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="155" priority="86" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="135" priority="86" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="154" priority="87" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="134" priority="87" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="153" priority="83" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="83" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="132" priority="84" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsText" dxfId="151" priority="80" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="131" priority="80" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="81" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="130" priority="81" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="149" priority="82" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="129" priority="82" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="148" priority="78" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="78" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="127" priority="79" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsText" dxfId="146" priority="75" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="126" priority="75" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="76" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="125" priority="76" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="77" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="124" priority="77" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="143" priority="73" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="73" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="74" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsText" dxfId="141" priority="70" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="121" priority="70" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="140" priority="71" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="120" priority="71" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="72" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="119" priority="72" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="138" priority="68" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="68" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="117" priority="69" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="containsText" dxfId="136" priority="65" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="116" priority="65" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="66" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="115" priority="66" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="67" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="114" priority="67" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="133" priority="63" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="63" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="64" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="containsText" dxfId="131" priority="60" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="111" priority="60" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="61" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="110" priority="61" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="62" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="109" priority="62" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="128" priority="58" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="58" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="107" priority="59" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="126" priority="56" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="56" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="105" priority="57" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="containsText" dxfId="124" priority="53" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="104" priority="53" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="54" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="103" priority="54" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="55" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="102" priority="55" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="121" priority="51" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="51" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="100" priority="52" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="containsText" dxfId="119" priority="48" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="99" priority="48" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="49" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="98" priority="49" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="50" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="97" priority="50" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="116" priority="46" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="46" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="47" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="containsText" dxfId="114" priority="43" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="94" priority="43" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="44" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="93" priority="44" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="45" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="92" priority="45" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="111" priority="41" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="41" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="42" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="containsText" dxfId="109" priority="38" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="89" priority="38" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="39" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="88" priority="39" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="40" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="87" priority="40" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="106" priority="36" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="36" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="37" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="containsText" dxfId="104" priority="33" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="84" priority="33" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="34" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="83" priority="34" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="35" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="82" priority="35" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="101" priority="31" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="31" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="32" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="containsText" dxfId="59" priority="28" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="79" priority="28" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="29" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="78" priority="29" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="30" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="77" priority="30" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="53" priority="26" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="26" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="27" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="containsText" dxfId="49" priority="23" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="74" priority="23" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="24" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="73" priority="24" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="25" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="72" priority="25" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="43" priority="21" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="21" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="22" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="containsText" dxfId="39" priority="18" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="69" priority="18" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="19" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="68" priority="19" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="20" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="67" priority="20" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="33" priority="16" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="16" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="17" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="containsText" dxfId="29" priority="13" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="64" priority="13" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="14" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="63" priority="14" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="15" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="62" priority="15" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="11" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="12" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="59" priority="8" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="58" priority="9" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="57" priority="10" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="6" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="7" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="54" priority="3" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="53" priority="4" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="52" priority="5" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>